<commit_message>
Updates to bulk order flow:   * Removed unneeded project_name from database and code   * Added order_count field to database to track order count instead of counting excel rows.   * Change bulk flow from tabbed view on step 2 to order_count on step 1 with bulk total price view.
</commit_message>
<xml_diff>
--- a/public/downloads/bulk_sample.xlsx
+++ b/public/downloads/bulk_sample.xlsx
@@ -19,93 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
-  <si>
-    <t>project_name</t>
-  </si>
-  <si>
-    <t>duedate</t>
-  </si>
-  <si>
-    <t>asset_type_id</t>
-  </si>
-  <si>
-    <t>wordcount</t>
-  </si>
-  <si>
-    <t>writer_level</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>content_title</t>
   </si>
   <si>
     <t>instructions</t>
-  </si>
-  <si>
-    <t>narrative_voice</t>
-  </si>
-  <si>
-    <t>target_audience</t>
-  </si>
-  <si>
-    <t>tone_of_writing</t>
-  </si>
-  <si>
-    <t>test 1</t>
-  </si>
-  <si>
-    <t>tbd</t>
-  </si>
-  <si>
-    <t>Second Person</t>
-  </si>
-  <si>
-    <t>Prospect Customers</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>First Person Plural</t>
-  </si>
-  <si>
-    <t>new blog 12.22.16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test 123. </t>
-  </si>
-  <si>
-    <t>First Person Singular</t>
-  </si>
-  <si>
-    <t>Customers</t>
-  </si>
-  <si>
-    <t>Business Formal</t>
-  </si>
-  <si>
-    <t>Journalistic</t>
-  </si>
-  <si>
-    <t>Extremely Informal</t>
-  </si>
-  <si>
-    <t>Sports Blog</t>
-  </si>
-  <si>
-    <t>Stay at home Mom blog</t>
-  </si>
-  <si>
-    <t>How to get your kids out of bed</t>
-  </si>
-  <si>
-    <t>Getting dressed and brushing teeth</t>
-  </si>
-  <si>
-    <t>Making breakfast for 4 kids</t>
-  </si>
-  <si>
-    <t>Top ten ways to get them dressed</t>
   </si>
 </sst>
 </file>
@@ -162,23 +81,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -508,249 +430,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="147.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1">
-        <v>42704</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>500</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1">
-        <v>42711</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2000</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1">
-        <v>42732</v>
-      </c>
-      <c r="C4">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>50</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1">
-        <v>42704</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>500</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1">
-        <v>42711</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>2000</v>
-      </c>
-      <c r="E6">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1">
-        <v>42732</v>
-      </c>
-      <c r="C7">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>50</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>